<commit_message>
Rediseño red parte 2 added vlans
</commit_message>
<xml_diff>
--- a/fol/UBALDE_Parch Panels - Esquema conexiones.xlsx
+++ b/fol/UBALDE_Parch Panels - Esquema conexiones.xlsx
@@ -1,15 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4F20289-642C-4B01-9C39-FFA11A9C7E02}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Kerjox\Repos\2h\fol\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D996570B-C6C0-44D8-A985-7F9ED4AD65CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{47CFAA2B-B6FE-4C8E-9BA2-DB30D79CCD5C}"/>
+    <workbookView xWindow="15" yWindow="15" windowWidth="38370" windowHeight="20970" activeTab="2" xr2:uid="{47CFAA2B-B6FE-4C8E-9BA2-DB30D79CCD5C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planta_Inferior" sheetId="2" r:id="rId1"/>
     <sheet name="Planta_Superior" sheetId="1" r:id="rId2"/>
+    <sheet name="VLANs" sheetId="3" r:id="rId3"/>
+    <sheet name="Static IPs" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -21,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="242">
   <si>
     <t>Patch Panel 3</t>
   </si>
@@ -492,13 +499,268 @@
   </si>
   <si>
     <t>Boca4 - B3</t>
+  </si>
+  <si>
+    <t>Demo_Area</t>
+  </si>
+  <si>
+    <t>Developers</t>
+  </si>
+  <si>
+    <t>Programers</t>
+  </si>
+  <si>
+    <t>Native-Trunk</t>
+  </si>
+  <si>
+    <t>Systems-administrators</t>
+  </si>
+  <si>
+    <t>Commercial</t>
+  </si>
+  <si>
+    <t>Accounting</t>
+  </si>
+  <si>
+    <t>Call-Center</t>
+  </si>
+  <si>
+    <t>R-H</t>
+  </si>
+  <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>Reception</t>
+  </si>
+  <si>
+    <t>Black-Hole</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>VLAN</t>
+  </si>
+  <si>
+    <t>Network IP</t>
+  </si>
+  <si>
+    <t>192.168.10.0/24</t>
+  </si>
+  <si>
+    <t>192.168.20.0/24</t>
+  </si>
+  <si>
+    <t>192.168.30.0/24</t>
+  </si>
+  <si>
+    <t>192.168.40.0/24</t>
+  </si>
+  <si>
+    <t>192.168.50.0/24</t>
+  </si>
+  <si>
+    <t>192.168.60.0/24</t>
+  </si>
+  <si>
+    <t>192.168.70.0/24</t>
+  </si>
+  <si>
+    <t>192.168.80.0/24</t>
+  </si>
+  <si>
+    <t>192.168.90.0/24</t>
+  </si>
+  <si>
+    <t>192.168.100.0/24</t>
+  </si>
+  <si>
+    <t>192.168.110.0/24</t>
+  </si>
+  <si>
+    <t>192.168.120.0/24</t>
+  </si>
+  <si>
+    <t>192.168.130.0/24</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>192.168.10.1</t>
+  </si>
+  <si>
+    <t>192.168.100.1</t>
+  </si>
+  <si>
+    <t>192.168.110.1</t>
+  </si>
+  <si>
+    <t>192.168.130.1</t>
+  </si>
+  <si>
+    <t>192.168.20.1</t>
+  </si>
+  <si>
+    <t>192.168.30.1</t>
+  </si>
+  <si>
+    <t>192.168.40.1</t>
+  </si>
+  <si>
+    <t>192.168.50.1</t>
+  </si>
+  <si>
+    <t>192.168.60.1</t>
+  </si>
+  <si>
+    <t>192.168.70.1</t>
+  </si>
+  <si>
+    <t>192.168.80.1</t>
+  </si>
+  <si>
+    <t>192.168.90.1</t>
+  </si>
+  <si>
+    <t>DMZ</t>
+  </si>
+  <si>
+    <t>192.168.200.0/24</t>
+  </si>
+  <si>
+    <t>192.168.200.1</t>
+  </si>
+  <si>
+    <t>Printers</t>
+  </si>
+  <si>
+    <t>Servers</t>
+  </si>
+  <si>
+    <t>192.168.150.0/24</t>
+  </si>
+  <si>
+    <t>192.168.150.1</t>
+  </si>
+  <si>
+    <t>DHCP</t>
+  </si>
+  <si>
+    <t>192.168.10.10 - 192.168.10.49</t>
+  </si>
+  <si>
+    <t>192.168.20.10 - 192.168.20.49</t>
+  </si>
+  <si>
+    <t>192.168.30.10 - 192.168.30.49</t>
+  </si>
+  <si>
+    <t>192.168.40.10 - 192.168.40.49</t>
+  </si>
+  <si>
+    <t>192.168.50.10 - 192.168.50.49</t>
+  </si>
+  <si>
+    <t>192.168.60.10 - 192.168.60.49</t>
+  </si>
+  <si>
+    <t>192.168.70.10 - 192.168.70.49</t>
+  </si>
+  <si>
+    <t>192.168.90.10 - 192.168.90.49</t>
+  </si>
+  <si>
+    <t>192.168.100.10 - 192.168.100.49</t>
+  </si>
+  <si>
+    <t>192.168.120.10 - 192.168.120.49</t>
+  </si>
+  <si>
+    <t>192.168.99.0/24</t>
+  </si>
+  <si>
+    <t>WiFi_Empleados</t>
+  </si>
+  <si>
+    <t>Router_Movistar</t>
+  </si>
+  <si>
+    <t>Switch_C1</t>
+  </si>
+  <si>
+    <t>Switch_C2</t>
+  </si>
+  <si>
+    <t>Switch_P1-1</t>
+  </si>
+  <si>
+    <t>Switch_P1-2</t>
+  </si>
+  <si>
+    <t>Switch_P1-3</t>
+  </si>
+  <si>
+    <t>Switch_p0-1</t>
+  </si>
+  <si>
+    <t>192.168.49.50</t>
+  </si>
+  <si>
+    <t>192.168.49.51</t>
+  </si>
+  <si>
+    <t>192.168.49.100</t>
+  </si>
+  <si>
+    <t>192.168.49.101</t>
+  </si>
+  <si>
+    <t>192.168.49.102</t>
+  </si>
+  <si>
+    <t>192.168.49.103</t>
+  </si>
+  <si>
+    <t>192.168.49.104</t>
+  </si>
+  <si>
+    <t>192.168.49.105</t>
+  </si>
+  <si>
+    <t>IP Address</t>
+  </si>
+  <si>
+    <t>Device Name</t>
+  </si>
+  <si>
+    <t>VLAN 49 - Management</t>
+  </si>
+  <si>
+    <t>HSRP</t>
+  </si>
+  <si>
+    <t>Router_Vodafone</t>
+  </si>
+  <si>
+    <t>Gateway</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>192.168.130.10 - 192.168.130.15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -524,6 +786,28 @@
       <b/>
       <i/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -616,7 +900,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -630,11 +914,190 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -645,6 +1108,32 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{93E6DCE9-8BA4-420E-BB3D-039C2EDE02DF}" name="Tabla1" displayName="Tabla1" ref="C5:H23" totalsRowShown="0" headerRowDxfId="2" dataDxfId="1">
+  <autoFilter ref="C5:H23" xr:uid="{93E6DCE9-8BA4-420E-BB3D-039C2EDE02DF}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{B1900C5F-ADF5-444B-A3E6-F889D88F02DC}" name="VLAN" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{70173B9A-8C3C-4CC0-B369-9F47495DD7E2}" name="Name" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{CE93E623-EABD-4E7D-8455-89684789B49F}" name="Network IP" dataDxfId="5"/>
+    <tableColumn id="4" xr3:uid="{A9D9A673-30F5-43AB-A71F-5988F5D62943}" name="Gateway" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{C4E2A420-D64C-431C-ABB1-A9DA3076B77E}" name="DHCP" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{381D94C1-DCB9-4DF8-B6CB-B475D6202ABD}" name="HSRP" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{988AAF32-4E74-45E7-A18C-52815099CE9F}" name="Tabla2" displayName="Tabla2" ref="D7:E15" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="D7:E15" xr:uid="{988AAF32-4E74-45E7-A18C-52815099CE9F}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{F715B4CA-C1BB-49AF-935B-062958289F77}" name="Device Name" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{72A46CE8-EA0A-4374-AAC3-53E877046E9A}" name="IP Address" dataDxfId="10"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium4" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1175,7 +1664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FD1E556-852C-4223-8EEF-59310559789A}">
   <dimension ref="A4:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
@@ -1718,4 +2207,514 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58442A95-5C1E-44BC-8F9B-AE10EBD2173D}">
+  <dimension ref="C5:H23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C5" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>169</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>239</v>
+      </c>
+      <c r="G5" s="11" t="s">
+        <v>206</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C6" s="12">
+        <v>10</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>207</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C7" s="12">
+        <v>20</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>208</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C8" s="12">
+        <v>30</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C9" s="12">
+        <v>40</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C10" s="12">
+        <v>49</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C11" s="12">
+        <v>50</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>211</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C12" s="12">
+        <v>60</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C13" s="12">
+        <v>70</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>196</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C14" s="12">
+        <v>80</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>179</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C15" s="12">
+        <v>90</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>165</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C16" s="12">
+        <v>99</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>217</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C17" s="12">
+        <v>100</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>215</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C18" s="12">
+        <v>110</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C19" s="12">
+        <v>120</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="E19" s="9" t="s">
+        <v>183</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>216</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C20" s="12">
+        <v>130</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C21" s="12">
+        <v>150</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="E21" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>205</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C22" s="12">
+        <v>200</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="C23" s="12">
+        <v>555</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>168</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="H23" s="9"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53660A50-DF82-4D92-9B22-5398741FD718}">
+  <dimension ref="D6:E15"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="6" spans="4:5" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D6" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="E6" s="10"/>
+    </row>
+    <row r="7" spans="4:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D7" s="9" t="s">
+        <v>235</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D8" s="9" t="s">
+        <v>219</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D9" s="9" t="s">
+        <v>238</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" spans="4:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D10" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="11" spans="4:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D11" s="9" t="s">
+        <v>221</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="12" spans="4:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D12" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="4:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D13" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="4:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D14" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="4:5" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="D15" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>233</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D6:E6"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>